<commit_message>
Added lessons to students folder
</commit_message>
<xml_diff>
--- a/data/iris.xlsx
+++ b/data/iris.xlsx
@@ -1,33 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Oblivion/Vault/MyDataScience/General_Assembly/dat11syd_admin/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="iris" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>sepal_length</t>
   </si>
@@ -56,25 +44,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,23 +74,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -113,44 +109,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -177,15 +173,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -212,7 +207,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -224,3164 +218,3194 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C2" t="n">
         <v>3.5</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>1.4</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>0.2</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>1.4</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>0.2</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>4.7</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>3.2</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>1.3</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>0.2</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C5" t="n">
         <v>3.1</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>1.5</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>0.2</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
         <v>3.6</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>1.4</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>0.2</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
         <v>5.4</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>3.9</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>1.7</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>0.4</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C8">
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C8" t="n">
         <v>3.4</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>1.4</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>0.3</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
         <v>3.4</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>1.5</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>0.2</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C10">
+      <c r="B10" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C10" t="n">
         <v>2.9</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>1.4</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>0.2</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C11">
+      <c r="B11" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C11" t="n">
         <v>3.1</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>1.5</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>0.1</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>5.4</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>3.7</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>1.5</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>0.2</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>4.8</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>3.4</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>1.6</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>0.2</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>4.8</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>1.4</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>0.1</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>4.3</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>3</v>
       </c>
-      <c r="D15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E15">
+      <c r="D15" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E15" t="n">
         <v>0.1</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>5.8</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>4</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>1.2</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>0.2</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>5.7</v>
       </c>
-      <c r="C17">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D17">
+      <c r="C17" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D17" t="n">
         <v>1.5</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>0.4</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>5.4</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>3.9</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>1.3</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>0.4</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C19">
+      <c r="B19" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C19" t="n">
         <v>3.5</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="n">
         <v>1.4</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>0.3</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>5.7</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="n">
         <v>3.8</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <v>1.7</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>0.3</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C21">
+      <c r="B21" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C21" t="n">
         <v>3.8</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="n">
         <v>1.5</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="n">
         <v>0.3</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>5.4</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="n">
         <v>3.4</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="n">
         <v>1.7</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>0.2</v>
       </c>
       <c r="F22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C23">
+      <c r="B23" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C23" t="n">
         <v>3.7</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="n">
         <v>1.5</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>0.4</v>
       </c>
       <c r="F23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C24">
+      <c r="B24" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C24" t="n">
         <v>3.6</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>1</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>0.2</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C25">
+      <c r="B25" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C25" t="n">
         <v>3.3</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>1.7</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>0.5</v>
       </c>
       <c r="F25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>4.8</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>3.4</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>1.9</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>0.2</v>
       </c>
       <c r="F26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27">
+      <c r="B27" t="n">
+        <v>5</v>
+      </c>
+      <c r="C27" t="n">
         <v>3</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>1.6</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>0.2</v>
       </c>
       <c r="F27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28">
+      <c r="B28" t="n">
+        <v>5</v>
+      </c>
+      <c r="C28" t="n">
         <v>3.4</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>1.6</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>0.4</v>
       </c>
       <c r="F28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>5.2</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="n">
         <v>3.5</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="n">
         <v>1.5</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>0.2</v>
       </c>
       <c r="F29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>5.2</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>3.4</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>1.4</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>0.2</v>
       </c>
       <c r="F30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>4.7</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>3.2</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>1.6</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>0.2</v>
       </c>
       <c r="F31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>4.8</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="n">
         <v>3.1</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="n">
         <v>1.6</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="n">
         <v>0.2</v>
       </c>
       <c r="F32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>5.4</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>3.4</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="n">
         <v>1.5</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>0.4</v>
       </c>
       <c r="F33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>5.2</v>
       </c>
-      <c r="C34">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D34">
+      <c r="C34" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D34" t="n">
         <v>1.5</v>
       </c>
-      <c r="E34">
+      <c r="E34" t="n">
         <v>0.1</v>
       </c>
       <c r="F34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="n">
         <v>5.5</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="n">
         <v>4.2</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="n">
         <v>1.4</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="n">
         <v>0.2</v>
       </c>
       <c r="F35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C36">
+      <c r="B36" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C36" t="n">
         <v>3.1</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="n">
         <v>1.5</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="n">
         <v>0.1</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="37" spans="1:6">
+      <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
+      <c r="B37" t="n">
+        <v>5</v>
+      </c>
+      <c r="C37" t="n">
         <v>3.2</v>
       </c>
-      <c r="D37">
+      <c r="D37" t="n">
         <v>1.2</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="n">
         <v>0.2</v>
       </c>
       <c r="F37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="n">
         <v>5.5</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="n">
         <v>3.5</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="n">
         <v>1.3</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="n">
         <v>0.2</v>
       </c>
       <c r="F38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C39">
+      <c r="B39" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C39" t="n">
         <v>3.1</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="n">
         <v>1.5</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="n">
         <v>0.1</v>
       </c>
       <c r="F39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C40">
+      <c r="B40" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C40" t="n">
         <v>3</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="n">
         <v>1.3</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="n">
         <v>0.2</v>
       </c>
       <c r="F40" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C41">
+      <c r="B41" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C41" t="n">
         <v>3.4</v>
       </c>
-      <c r="D41">
+      <c r="D41" t="n">
         <v>1.5</v>
       </c>
-      <c r="E41">
+      <c r="E41" t="n">
         <v>0.2</v>
       </c>
       <c r="F41" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-      <c r="C42">
+      <c r="B42" t="n">
+        <v>5</v>
+      </c>
+      <c r="C42" t="n">
         <v>3.5</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="n">
         <v>1.3</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="n">
         <v>0.3</v>
       </c>
       <c r="F42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
+    <row r="43" spans="1:6">
+      <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="n">
         <v>4.5</v>
       </c>
-      <c r="C43">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D43">
+      <c r="C43" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D43" t="n">
         <v>1.3</v>
       </c>
-      <c r="E43">
+      <c r="E43" t="n">
         <v>0.3</v>
       </c>
       <c r="F43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="44" spans="1:6">
+      <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C44">
+      <c r="B44" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C44" t="n">
         <v>3.2</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="n">
         <v>1.3</v>
       </c>
-      <c r="E44">
+      <c r="E44" t="n">
         <v>0.2</v>
       </c>
       <c r="F44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
+    <row r="45" spans="1:6">
+      <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
-      <c r="C45">
+      <c r="B45" t="n">
+        <v>5</v>
+      </c>
+      <c r="C45" t="n">
         <v>3.5</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="n">
         <v>1.6</v>
       </c>
-      <c r="E45">
+      <c r="E45" t="n">
         <v>0.6</v>
       </c>
       <c r="F45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
+    <row r="46" spans="1:6">
+      <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C46">
+      <c r="B46" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C46" t="n">
         <v>3.8</v>
       </c>
-      <c r="D46">
+      <c r="D46" t="n">
         <v>1.9</v>
       </c>
-      <c r="E46">
+      <c r="E46" t="n">
         <v>0.4</v>
       </c>
       <c r="F46" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
+    <row r="47" spans="1:6">
+      <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47">
+      <c r="B47" t="n">
         <v>4.8</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="n">
         <v>3</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="n">
         <v>1.4</v>
       </c>
-      <c r="E47">
+      <c r="E47" t="n">
         <v>0.3</v>
       </c>
       <c r="F47" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
+    <row r="48" spans="1:6">
+      <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C48">
+      <c r="B48" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C48" t="n">
         <v>3.8</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="n">
         <v>1.6</v>
       </c>
-      <c r="E48">
+      <c r="E48" t="n">
         <v>0.2</v>
       </c>
       <c r="F48" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49">
+    <row r="49" spans="1:6">
+      <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C49">
+      <c r="B49" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C49" t="n">
         <v>3.2</v>
       </c>
-      <c r="D49">
+      <c r="D49" t="n">
         <v>1.4</v>
       </c>
-      <c r="E49">
+      <c r="E49" t="n">
         <v>0.2</v>
       </c>
       <c r="F49" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50">
+    <row r="50" spans="1:6">
+      <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B50" t="n">
         <v>5.3</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="n">
         <v>3.7</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="n">
         <v>1.5</v>
       </c>
-      <c r="E50">
+      <c r="E50" t="n">
         <v>0.2</v>
       </c>
       <c r="F50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51">
+    <row r="51" spans="1:6">
+      <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51">
-        <v>5</v>
-      </c>
-      <c r="C51">
+      <c r="B51" t="n">
+        <v>5</v>
+      </c>
+      <c r="C51" t="n">
         <v>3.3</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="n">
         <v>1.4</v>
       </c>
-      <c r="E51">
+      <c r="E51" t="n">
         <v>0.2</v>
       </c>
       <c r="F51" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52">
+    <row r="52" spans="1:6">
+      <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52">
-        <v>7</v>
-      </c>
-      <c r="C52">
+      <c r="B52" t="n">
+        <v>7</v>
+      </c>
+      <c r="C52" t="n">
         <v>3.2</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="n">
         <v>4.7</v>
       </c>
-      <c r="E52">
+      <c r="E52" t="n">
         <v>1.4</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53">
+    <row r="53" spans="1:6">
+      <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53">
+      <c r="B53" t="n">
         <v>6.4</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="n">
         <v>3.2</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="n">
         <v>4.5</v>
       </c>
-      <c r="E53">
+      <c r="E53" t="n">
         <v>1.5</v>
       </c>
       <c r="F53" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54">
+    <row r="54" spans="1:6">
+      <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54">
+      <c r="B54" t="n">
         <v>6.9</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="n">
         <v>3.1</v>
       </c>
-      <c r="D54">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E54">
+      <c r="D54" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E54" t="n">
         <v>1.5</v>
       </c>
       <c r="F54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55">
+    <row r="55" spans="1:6">
+      <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55">
+      <c r="B55" t="n">
         <v>5.5</v>
       </c>
-      <c r="C55">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D55">
+      <c r="C55" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D55" t="n">
         <v>4</v>
       </c>
-      <c r="E55">
+      <c r="E55" t="n">
         <v>1.3</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56">
+    <row r="56" spans="1:6">
+      <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56">
+      <c r="B56" t="n">
         <v>6.5</v>
       </c>
-      <c r="C56">
+      <c r="C56" t="n">
         <v>2.8</v>
       </c>
-      <c r="D56">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E56">
+      <c r="D56" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E56" t="n">
         <v>1.5</v>
       </c>
       <c r="F56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57">
+    <row r="57" spans="1:6">
+      <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57">
+      <c r="B57" t="n">
         <v>5.7</v>
       </c>
-      <c r="C57">
+      <c r="C57" t="n">
         <v>2.8</v>
       </c>
-      <c r="D57">
+      <c r="D57" t="n">
         <v>4.5</v>
       </c>
-      <c r="E57">
+      <c r="E57" t="n">
         <v>1.3</v>
       </c>
       <c r="F57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58">
+    <row r="58" spans="1:6">
+      <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58">
+      <c r="B58" t="n">
         <v>6.3</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="n">
         <v>3.3</v>
       </c>
-      <c r="D58">
+      <c r="D58" t="n">
         <v>4.7</v>
       </c>
-      <c r="E58">
+      <c r="E58" t="n">
         <v>1.6</v>
       </c>
       <c r="F58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59">
+    <row r="59" spans="1:6">
+      <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C59">
+      <c r="B59" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C59" t="n">
         <v>2.4</v>
       </c>
-      <c r="D59">
+      <c r="D59" t="n">
         <v>3.3</v>
       </c>
-      <c r="E59">
+      <c r="E59" t="n">
         <v>1</v>
       </c>
       <c r="F59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60">
+    <row r="60" spans="1:6">
+      <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60">
+      <c r="B60" t="n">
         <v>6.6</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="n">
         <v>2.9</v>
       </c>
-      <c r="D60">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E60">
+      <c r="D60" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E60" t="n">
         <v>1.3</v>
       </c>
       <c r="F60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61">
+    <row r="61" spans="1:6">
+      <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B61">
+      <c r="B61" t="n">
         <v>5.2</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="n">
         <v>2.7</v>
       </c>
-      <c r="D61">
+      <c r="D61" t="n">
         <v>3.9</v>
       </c>
-      <c r="E61">
+      <c r="E61" t="n">
         <v>1.4</v>
       </c>
       <c r="F61" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62">
+    <row r="62" spans="1:6">
+      <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62">
-        <v>5</v>
-      </c>
-      <c r="C62">
+      <c r="B62" t="n">
+        <v>5</v>
+      </c>
+      <c r="C62" t="n">
         <v>2</v>
       </c>
-      <c r="D62">
+      <c r="D62" t="n">
         <v>3.5</v>
       </c>
-      <c r="E62">
+      <c r="E62" t="n">
         <v>1</v>
       </c>
       <c r="F62" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63">
+    <row r="63" spans="1:6">
+      <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63">
+      <c r="B63" t="n">
         <v>5.9</v>
       </c>
-      <c r="C63">
+      <c r="C63" t="n">
         <v>3</v>
       </c>
-      <c r="D63">
+      <c r="D63" t="n">
         <v>4.2</v>
       </c>
-      <c r="E63">
+      <c r="E63" t="n">
         <v>1.5</v>
       </c>
       <c r="F63" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64">
+    <row r="64" spans="1:6">
+      <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64">
-        <v>6</v>
-      </c>
-      <c r="C64">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D64">
+      <c r="B64" t="n">
+        <v>6</v>
+      </c>
+      <c r="C64" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D64" t="n">
         <v>4</v>
       </c>
-      <c r="E64">
+      <c r="E64" t="n">
         <v>1</v>
       </c>
       <c r="F64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65">
+    <row r="65" spans="1:6">
+      <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65">
+      <c r="B65" t="n">
         <v>6.1</v>
       </c>
-      <c r="C65">
+      <c r="C65" t="n">
         <v>2.9</v>
       </c>
-      <c r="D65">
+      <c r="D65" t="n">
         <v>4.7</v>
       </c>
-      <c r="E65">
+      <c r="E65" t="n">
         <v>1.4</v>
       </c>
       <c r="F65" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66">
+    <row r="66" spans="1:6">
+      <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B66">
+      <c r="B66" t="n">
         <v>5.6</v>
       </c>
-      <c r="C66">
+      <c r="C66" t="n">
         <v>2.9</v>
       </c>
-      <c r="D66">
+      <c r="D66" t="n">
         <v>3.6</v>
       </c>
-      <c r="E66">
+      <c r="E66" t="n">
         <v>1.3</v>
       </c>
       <c r="F66" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67">
+    <row r="67" spans="1:6">
+      <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67">
+      <c r="B67" t="n">
         <v>6.7</v>
       </c>
-      <c r="C67">
+      <c r="C67" t="n">
         <v>3.1</v>
       </c>
-      <c r="D67">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E67">
+      <c r="D67" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E67" t="n">
         <v>1.4</v>
       </c>
       <c r="F67" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68">
+    <row r="68" spans="1:6">
+      <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68">
+      <c r="B68" t="n">
         <v>5.6</v>
       </c>
-      <c r="C68">
+      <c r="C68" t="n">
         <v>3</v>
       </c>
-      <c r="D68">
+      <c r="D68" t="n">
         <v>4.5</v>
       </c>
-      <c r="E68">
+      <c r="E68" t="n">
         <v>1.5</v>
       </c>
       <c r="F68" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69">
+    <row r="69" spans="1:6">
+      <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69">
+      <c r="B69" t="n">
         <v>5.8</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="n">
         <v>2.7</v>
       </c>
-      <c r="D69">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E69">
+      <c r="D69" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E69" t="n">
         <v>1</v>
       </c>
       <c r="F69" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70">
+    <row r="70" spans="1:6">
+      <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70">
+      <c r="B70" t="n">
         <v>6.2</v>
       </c>
-      <c r="C70">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D70">
+      <c r="C70" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D70" t="n">
         <v>4.5</v>
       </c>
-      <c r="E70">
+      <c r="E70" t="n">
         <v>1.5</v>
       </c>
       <c r="F70" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71">
+    <row r="71" spans="1:6">
+      <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B71">
+      <c r="B71" t="n">
         <v>5.6</v>
       </c>
-      <c r="C71">
+      <c r="C71" t="n">
         <v>2.5</v>
       </c>
-      <c r="D71">
+      <c r="D71" t="n">
         <v>3.9</v>
       </c>
-      <c r="E71">
-        <v>1.1000000000000001</v>
+      <c r="E71" t="n">
+        <v>1.1</v>
       </c>
       <c r="F71" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72">
+    <row r="72" spans="1:6">
+      <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B72">
+      <c r="B72" t="n">
         <v>5.9</v>
       </c>
-      <c r="C72">
+      <c r="C72" t="n">
         <v>3.2</v>
       </c>
-      <c r="D72">
+      <c r="D72" t="n">
         <v>4.8</v>
       </c>
-      <c r="E72">
+      <c r="E72" t="n">
         <v>1.8</v>
       </c>
       <c r="F72" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73">
+    <row r="73" spans="1:6">
+      <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B73">
+      <c r="B73" t="n">
         <v>6.1</v>
       </c>
-      <c r="C73">
+      <c r="C73" t="n">
         <v>2.8</v>
       </c>
-      <c r="D73">
+      <c r="D73" t="n">
         <v>4</v>
       </c>
-      <c r="E73">
+      <c r="E73" t="n">
         <v>1.3</v>
       </c>
       <c r="F73" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74">
+    <row r="74" spans="1:6">
+      <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B74">
+      <c r="B74" t="n">
         <v>6.3</v>
       </c>
-      <c r="C74">
+      <c r="C74" t="n">
         <v>2.5</v>
       </c>
-      <c r="D74">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E74">
+      <c r="D74" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E74" t="n">
         <v>1.5</v>
       </c>
       <c r="F74" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75">
+    <row r="75" spans="1:6">
+      <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B75">
+      <c r="B75" t="n">
         <v>6.1</v>
       </c>
-      <c r="C75">
+      <c r="C75" t="n">
         <v>2.8</v>
       </c>
-      <c r="D75">
+      <c r="D75" t="n">
         <v>4.7</v>
       </c>
-      <c r="E75">
+      <c r="E75" t="n">
         <v>1.2</v>
       </c>
       <c r="F75" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76">
+    <row r="76" spans="1:6">
+      <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B76">
+      <c r="B76" t="n">
         <v>6.4</v>
       </c>
-      <c r="C76">
+      <c r="C76" t="n">
         <v>2.9</v>
       </c>
-      <c r="D76">
+      <c r="D76" t="n">
         <v>4.3</v>
       </c>
-      <c r="E76">
+      <c r="E76" t="n">
         <v>1.3</v>
       </c>
       <c r="F76" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77">
+    <row r="77" spans="1:6">
+      <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B77">
+      <c r="B77" t="n">
         <v>6.6</v>
       </c>
-      <c r="C77">
+      <c r="C77" t="n">
         <v>3</v>
       </c>
-      <c r="D77">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E77">
+      <c r="D77" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E77" t="n">
         <v>1.4</v>
       </c>
       <c r="F77" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78">
+    <row r="78" spans="1:6">
+      <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B78">
+      <c r="B78" t="n">
         <v>6.8</v>
       </c>
-      <c r="C78">
+      <c r="C78" t="n">
         <v>2.8</v>
       </c>
-      <c r="D78">
+      <c r="D78" t="n">
         <v>4.8</v>
       </c>
-      <c r="E78">
+      <c r="E78" t="n">
         <v>1.4</v>
       </c>
       <c r="F78" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79">
+    <row r="79" spans="1:6">
+      <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B79">
+      <c r="B79" t="n">
         <v>6.7</v>
       </c>
-      <c r="C79">
+      <c r="C79" t="n">
         <v>3</v>
       </c>
-      <c r="D79">
-        <v>5</v>
-      </c>
-      <c r="E79">
+      <c r="D79" t="n">
+        <v>5</v>
+      </c>
+      <c r="E79" t="n">
         <v>1.7</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80">
+    <row r="80" spans="1:6">
+      <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B80">
-        <v>6</v>
-      </c>
-      <c r="C80">
+      <c r="B80" t="n">
+        <v>6</v>
+      </c>
+      <c r="C80" t="n">
         <v>2.9</v>
       </c>
-      <c r="D80">
+      <c r="D80" t="n">
         <v>4.5</v>
       </c>
-      <c r="E80">
+      <c r="E80" t="n">
         <v>1.5</v>
       </c>
       <c r="F80" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81">
+    <row r="81" spans="1:6">
+      <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81">
+      <c r="B81" t="n">
         <v>5.7</v>
       </c>
-      <c r="C81">
+      <c r="C81" t="n">
         <v>2.6</v>
       </c>
-      <c r="D81">
+      <c r="D81" t="n">
         <v>3.5</v>
       </c>
-      <c r="E81">
+      <c r="E81" t="n">
         <v>1</v>
       </c>
       <c r="F81" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82">
+    <row r="82" spans="1:6">
+      <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82">
+      <c r="B82" t="n">
         <v>5.5</v>
       </c>
-      <c r="C82">
+      <c r="C82" t="n">
         <v>2.4</v>
       </c>
-      <c r="D82">
+      <c r="D82" t="n">
         <v>3.8</v>
       </c>
-      <c r="E82">
-        <v>1.1000000000000001</v>
+      <c r="E82" t="n">
+        <v>1.1</v>
       </c>
       <c r="F82" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83">
+    <row r="83" spans="1:6">
+      <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B83">
+      <c r="B83" t="n">
         <v>5.5</v>
       </c>
-      <c r="C83">
+      <c r="C83" t="n">
         <v>2.4</v>
       </c>
-      <c r="D83">
+      <c r="D83" t="n">
         <v>3.7</v>
       </c>
-      <c r="E83">
+      <c r="E83" t="n">
         <v>1</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84">
+    <row r="84" spans="1:6">
+      <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84">
+      <c r="B84" t="n">
         <v>5.8</v>
       </c>
-      <c r="C84">
+      <c r="C84" t="n">
         <v>2.7</v>
       </c>
-      <c r="D84">
+      <c r="D84" t="n">
         <v>3.9</v>
       </c>
-      <c r="E84">
+      <c r="E84" t="n">
         <v>1.2</v>
       </c>
       <c r="F84" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85">
+    <row r="85" spans="1:6">
+      <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85">
-        <v>6</v>
-      </c>
-      <c r="C85">
+      <c r="B85" t="n">
+        <v>6</v>
+      </c>
+      <c r="C85" t="n">
         <v>2.7</v>
       </c>
-      <c r="D85">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E85">
+      <c r="D85" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E85" t="n">
         <v>1.6</v>
       </c>
       <c r="F85" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86">
+    <row r="86" spans="1:6">
+      <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B86">
+      <c r="B86" t="n">
         <v>5.4</v>
       </c>
-      <c r="C86">
+      <c r="C86" t="n">
         <v>3</v>
       </c>
-      <c r="D86">
+      <c r="D86" t="n">
         <v>4.5</v>
       </c>
-      <c r="E86">
+      <c r="E86" t="n">
         <v>1.5</v>
       </c>
       <c r="F86" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87">
+    <row r="87" spans="1:6">
+      <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87">
-        <v>6</v>
-      </c>
-      <c r="C87">
+      <c r="B87" t="n">
+        <v>6</v>
+      </c>
+      <c r="C87" t="n">
         <v>3.4</v>
       </c>
-      <c r="D87">
+      <c r="D87" t="n">
         <v>4.5</v>
       </c>
-      <c r="E87">
+      <c r="E87" t="n">
         <v>1.6</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88">
+    <row r="88" spans="1:6">
+      <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B88">
+      <c r="B88" t="n">
         <v>6.7</v>
       </c>
-      <c r="C88">
+      <c r="C88" t="n">
         <v>3.1</v>
       </c>
-      <c r="D88">
+      <c r="D88" t="n">
         <v>4.7</v>
       </c>
-      <c r="E88">
+      <c r="E88" t="n">
         <v>1.5</v>
       </c>
       <c r="F88" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89">
+    <row r="89" spans="1:6">
+      <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B89">
+      <c r="B89" t="n">
         <v>6.3</v>
       </c>
-      <c r="C89">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D89">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E89">
+      <c r="C89" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D89" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E89" t="n">
         <v>1.3</v>
       </c>
       <c r="F89" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90">
+    <row r="90" spans="1:6">
+      <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90">
+      <c r="B90" t="n">
         <v>5.6</v>
       </c>
-      <c r="C90">
+      <c r="C90" t="n">
         <v>3</v>
       </c>
-      <c r="D90">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E90">
+      <c r="D90" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E90" t="n">
         <v>1.3</v>
       </c>
       <c r="F90" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91">
+    <row r="91" spans="1:6">
+      <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B91">
+      <c r="B91" t="n">
         <v>5.5</v>
       </c>
-      <c r="C91">
+      <c r="C91" t="n">
         <v>2.5</v>
       </c>
-      <c r="D91">
+      <c r="D91" t="n">
         <v>4</v>
       </c>
-      <c r="E91">
+      <c r="E91" t="n">
         <v>1.3</v>
       </c>
       <c r="F91" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92">
+    <row r="92" spans="1:6">
+      <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B92">
+      <c r="B92" t="n">
         <v>5.5</v>
       </c>
-      <c r="C92">
+      <c r="C92" t="n">
         <v>2.6</v>
       </c>
-      <c r="D92">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E92">
+      <c r="D92" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E92" t="n">
         <v>1.2</v>
       </c>
       <c r="F92" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93">
+    <row r="93" spans="1:6">
+      <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93">
+      <c r="B93" t="n">
         <v>6.1</v>
       </c>
-      <c r="C93">
+      <c r="C93" t="n">
         <v>3</v>
       </c>
-      <c r="D93">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E93">
+      <c r="D93" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E93" t="n">
         <v>1.4</v>
       </c>
       <c r="F93" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94">
+    <row r="94" spans="1:6">
+      <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94">
+      <c r="B94" t="n">
         <v>5.8</v>
       </c>
-      <c r="C94">
+      <c r="C94" t="n">
         <v>2.6</v>
       </c>
-      <c r="D94">
+      <c r="D94" t="n">
         <v>4</v>
       </c>
-      <c r="E94">
+      <c r="E94" t="n">
         <v>1.2</v>
       </c>
       <c r="F94" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95">
+    <row r="95" spans="1:6">
+      <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B95">
-        <v>5</v>
-      </c>
-      <c r="C95">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D95">
+      <c r="B95" t="n">
+        <v>5</v>
+      </c>
+      <c r="C95" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D95" t="n">
         <v>3.3</v>
       </c>
-      <c r="E95">
+      <c r="E95" t="n">
         <v>1</v>
       </c>
       <c r="F95" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96">
+    <row r="96" spans="1:6">
+      <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B96">
+      <c r="B96" t="n">
         <v>5.6</v>
       </c>
-      <c r="C96">
+      <c r="C96" t="n">
         <v>2.7</v>
       </c>
-      <c r="D96">
+      <c r="D96" t="n">
         <v>4.2</v>
       </c>
-      <c r="E96">
+      <c r="E96" t="n">
         <v>1.3</v>
       </c>
       <c r="F96" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97">
+    <row r="97" spans="1:6">
+      <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B97">
+      <c r="B97" t="n">
         <v>5.7</v>
       </c>
-      <c r="C97">
+      <c r="C97" t="n">
         <v>3</v>
       </c>
-      <c r="D97">
+      <c r="D97" t="n">
         <v>4.2</v>
       </c>
-      <c r="E97">
+      <c r="E97" t="n">
         <v>1.2</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98">
+    <row r="98" spans="1:6">
+      <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98">
+      <c r="B98" t="n">
         <v>5.7</v>
       </c>
-      <c r="C98">
+      <c r="C98" t="n">
         <v>2.9</v>
       </c>
-      <c r="D98">
+      <c r="D98" t="n">
         <v>4.2</v>
       </c>
-      <c r="E98">
+      <c r="E98" t="n">
         <v>1.3</v>
       </c>
       <c r="F98" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99">
+    <row r="99" spans="1:6">
+      <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B99">
+      <c r="B99" t="n">
         <v>6.2</v>
       </c>
-      <c r="C99">
+      <c r="C99" t="n">
         <v>2.9</v>
       </c>
-      <c r="D99">
+      <c r="D99" t="n">
         <v>4.3</v>
       </c>
-      <c r="E99">
+      <c r="E99" t="n">
         <v>1.3</v>
       </c>
       <c r="F99" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100">
+    <row r="100" spans="1:6">
+      <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B100">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C100">
+      <c r="B100" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C100" t="n">
         <v>2.5</v>
       </c>
-      <c r="D100">
+      <c r="D100" t="n">
         <v>3</v>
       </c>
-      <c r="E100">
-        <v>1.1000000000000001</v>
+      <c r="E100" t="n">
+        <v>1.1</v>
       </c>
       <c r="F100" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101">
+    <row r="101" spans="1:6">
+      <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B101">
+      <c r="B101" t="n">
         <v>5.7</v>
       </c>
-      <c r="C101">
+      <c r="C101" t="n">
         <v>2.8</v>
       </c>
-      <c r="D101">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E101">
+      <c r="D101" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E101" t="n">
         <v>1.3</v>
       </c>
       <c r="F101" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102">
+    <row r="102" spans="1:6">
+      <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B102">
+      <c r="B102" t="n">
         <v>6.3</v>
       </c>
-      <c r="C102">
+      <c r="C102" t="n">
         <v>3.3</v>
       </c>
-      <c r="D102">
-        <v>6</v>
-      </c>
-      <c r="E102">
+      <c r="D102" t="n">
+        <v>6</v>
+      </c>
+      <c r="E102" t="n">
         <v>2.5</v>
       </c>
       <c r="F102" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103">
+    <row r="103" spans="1:6">
+      <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B103">
+      <c r="B103" t="n">
         <v>5.8</v>
       </c>
-      <c r="C103">
+      <c r="C103" t="n">
         <v>2.7</v>
       </c>
-      <c r="D103">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E103">
+      <c r="D103" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E103" t="n">
         <v>1.9</v>
       </c>
       <c r="F103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104">
+    <row r="104" spans="1:6">
+      <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B104">
+      <c r="B104" t="n">
         <v>7.1</v>
       </c>
-      <c r="C104">
+      <c r="C104" t="n">
         <v>3</v>
       </c>
-      <c r="D104">
+      <c r="D104" t="n">
         <v>5.9</v>
       </c>
-      <c r="E104">
+      <c r="E104" t="n">
         <v>2.1</v>
       </c>
       <c r="F104" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105">
+    <row r="105" spans="1:6">
+      <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B105">
+      <c r="B105" t="n">
         <v>6.3</v>
       </c>
-      <c r="C105">
+      <c r="C105" t="n">
         <v>2.9</v>
       </c>
-      <c r="D105">
+      <c r="D105" t="n">
         <v>5.6</v>
       </c>
-      <c r="E105">
+      <c r="E105" t="n">
         <v>1.8</v>
       </c>
       <c r="F105" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106">
+    <row r="106" spans="1:6">
+      <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B106">
+      <c r="B106" t="n">
         <v>6.5</v>
       </c>
-      <c r="C106">
+      <c r="C106" t="n">
         <v>3</v>
       </c>
-      <c r="D106">
+      <c r="D106" t="n">
         <v>5.8</v>
       </c>
-      <c r="E106">
-        <v>2.2000000000000002</v>
+      <c r="E106" t="n">
+        <v>2.2</v>
       </c>
       <c r="F106" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107">
+    <row r="107" spans="1:6">
+      <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="B107">
+      <c r="B107" t="n">
         <v>7.6</v>
       </c>
-      <c r="C107">
+      <c r="C107" t="n">
         <v>3</v>
       </c>
-      <c r="D107">
+      <c r="D107" t="n">
         <v>6.6</v>
       </c>
-      <c r="E107">
+      <c r="E107" t="n">
         <v>2.1</v>
       </c>
       <c r="F107" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108">
+    <row r="108" spans="1:6">
+      <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="B108">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C108">
+      <c r="B108" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C108" t="n">
         <v>2.5</v>
       </c>
-      <c r="D108">
+      <c r="D108" t="n">
         <v>4.5</v>
       </c>
-      <c r="E108">
+      <c r="E108" t="n">
         <v>1.7</v>
       </c>
       <c r="F108" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109">
+    <row r="109" spans="1:6">
+      <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="B109">
+      <c r="B109" t="n">
         <v>7.3</v>
       </c>
-      <c r="C109">
+      <c r="C109" t="n">
         <v>2.9</v>
       </c>
-      <c r="D109">
+      <c r="D109" t="n">
         <v>6.3</v>
       </c>
-      <c r="E109">
+      <c r="E109" t="n">
         <v>1.8</v>
       </c>
       <c r="F109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110">
+    <row r="110" spans="1:6">
+      <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="B110">
+      <c r="B110" t="n">
         <v>6.7</v>
       </c>
-      <c r="C110">
+      <c r="C110" t="n">
         <v>2.5</v>
       </c>
-      <c r="D110">
+      <c r="D110" t="n">
         <v>5.8</v>
       </c>
-      <c r="E110">
+      <c r="E110" t="n">
         <v>1.8</v>
       </c>
       <c r="F110" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111">
+    <row r="111" spans="1:6">
+      <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="B111">
+      <c r="B111" t="n">
         <v>7.2</v>
       </c>
-      <c r="C111">
+      <c r="C111" t="n">
         <v>3.6</v>
       </c>
-      <c r="D111">
+      <c r="D111" t="n">
         <v>6.1</v>
       </c>
-      <c r="E111">
+      <c r="E111" t="n">
         <v>2.5</v>
       </c>
       <c r="F111" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112">
+    <row r="112" spans="1:6">
+      <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="B112">
+      <c r="B112" t="n">
         <v>6.5</v>
       </c>
-      <c r="C112">
+      <c r="C112" t="n">
         <v>3.2</v>
       </c>
-      <c r="D112">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E112">
+      <c r="D112" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E112" t="n">
         <v>2</v>
       </c>
       <c r="F112" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113">
+    <row r="113" spans="1:6">
+      <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="B113">
+      <c r="B113" t="n">
         <v>6.4</v>
       </c>
-      <c r="C113">
+      <c r="C113" t="n">
         <v>2.7</v>
       </c>
-      <c r="D113">
+      <c r="D113" t="n">
         <v>5.3</v>
       </c>
-      <c r="E113">
+      <c r="E113" t="n">
         <v>1.9</v>
       </c>
       <c r="F113" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114">
+    <row r="114" spans="1:6">
+      <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="B114">
+      <c r="B114" t="n">
         <v>6.8</v>
       </c>
-      <c r="C114">
+      <c r="C114" t="n">
         <v>3</v>
       </c>
-      <c r="D114">
+      <c r="D114" t="n">
         <v>5.5</v>
       </c>
-      <c r="E114">
+      <c r="E114" t="n">
         <v>2.1</v>
       </c>
       <c r="F114" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115">
+    <row r="115" spans="1:6">
+      <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="B115">
+      <c r="B115" t="n">
         <v>5.7</v>
       </c>
-      <c r="C115">
+      <c r="C115" t="n">
         <v>2.5</v>
       </c>
-      <c r="D115">
-        <v>5</v>
-      </c>
-      <c r="E115">
+      <c r="D115" t="n">
+        <v>5</v>
+      </c>
+      <c r="E115" t="n">
         <v>2</v>
       </c>
       <c r="F115" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116">
+    <row r="116" spans="1:6">
+      <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="B116">
+      <c r="B116" t="n">
         <v>5.8</v>
       </c>
-      <c r="C116">
+      <c r="C116" t="n">
         <v>2.8</v>
       </c>
-      <c r="D116">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E116">
+      <c r="D116" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E116" t="n">
         <v>2.4</v>
       </c>
       <c r="F116" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117">
+    <row r="117" spans="1:6">
+      <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B117">
+      <c r="B117" t="n">
         <v>6.4</v>
       </c>
-      <c r="C117">
+      <c r="C117" t="n">
         <v>3.2</v>
       </c>
-      <c r="D117">
+      <c r="D117" t="n">
         <v>5.3</v>
       </c>
-      <c r="E117">
-        <v>2.2999999999999998</v>
+      <c r="E117" t="n">
+        <v>2.3</v>
       </c>
       <c r="F117" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118">
+    <row r="118" spans="1:6">
+      <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B118">
+      <c r="B118" t="n">
         <v>6.5</v>
       </c>
-      <c r="C118">
+      <c r="C118" t="n">
         <v>3</v>
       </c>
-      <c r="D118">
+      <c r="D118" t="n">
         <v>5.5</v>
       </c>
-      <c r="E118">
+      <c r="E118" t="n">
         <v>1.8</v>
       </c>
       <c r="F118" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119">
+    <row r="119" spans="1:6">
+      <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="B119">
+      <c r="B119" t="n">
         <v>7.7</v>
       </c>
-      <c r="C119">
+      <c r="C119" t="n">
         <v>3.8</v>
       </c>
-      <c r="D119">
+      <c r="D119" t="n">
         <v>6.7</v>
       </c>
-      <c r="E119">
-        <v>2.2000000000000002</v>
+      <c r="E119" t="n">
+        <v>2.2</v>
       </c>
       <c r="F119" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120">
+    <row r="120" spans="1:6">
+      <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="B120">
+      <c r="B120" t="n">
         <v>7.7</v>
       </c>
-      <c r="C120">
+      <c r="C120" t="n">
         <v>2.6</v>
       </c>
-      <c r="D120">
+      <c r="D120" t="n">
         <v>6.9</v>
       </c>
-      <c r="E120">
-        <v>2.2999999999999998</v>
+      <c r="E120" t="n">
+        <v>2.3</v>
       </c>
       <c r="F120" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121">
+    <row r="121" spans="1:6">
+      <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="B121">
-        <v>6</v>
-      </c>
-      <c r="C121">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D121">
-        <v>5</v>
-      </c>
-      <c r="E121">
+      <c r="B121" t="n">
+        <v>6</v>
+      </c>
+      <c r="C121" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D121" t="n">
+        <v>5</v>
+      </c>
+      <c r="E121" t="n">
         <v>1.5</v>
       </c>
       <c r="F121" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122">
+    <row r="122" spans="1:6">
+      <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B122">
+      <c r="B122" t="n">
         <v>6.9</v>
       </c>
-      <c r="C122">
+      <c r="C122" t="n">
         <v>3.2</v>
       </c>
-      <c r="D122">
+      <c r="D122" t="n">
         <v>5.7</v>
       </c>
-      <c r="E122">
-        <v>2.2999999999999998</v>
+      <c r="E122" t="n">
+        <v>2.3</v>
       </c>
       <c r="F122" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123">
+    <row r="123" spans="1:6">
+      <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="B123">
+      <c r="B123" t="n">
         <v>5.6</v>
       </c>
-      <c r="C123">
+      <c r="C123" t="n">
         <v>2.8</v>
       </c>
-      <c r="D123">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E123">
+      <c r="D123" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E123" t="n">
         <v>2</v>
       </c>
       <c r="F123" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124">
+    <row r="124" spans="1:6">
+      <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="B124">
+      <c r="B124" t="n">
         <v>7.7</v>
       </c>
-      <c r="C124">
+      <c r="C124" t="n">
         <v>2.8</v>
       </c>
-      <c r="D124">
+      <c r="D124" t="n">
         <v>6.7</v>
       </c>
-      <c r="E124">
+      <c r="E124" t="n">
         <v>2</v>
       </c>
       <c r="F124" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125">
+    <row r="125" spans="1:6">
+      <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="B125">
+      <c r="B125" t="n">
         <v>6.3</v>
       </c>
-      <c r="C125">
+      <c r="C125" t="n">
         <v>2.7</v>
       </c>
-      <c r="D125">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E125">
+      <c r="D125" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E125" t="n">
         <v>1.8</v>
       </c>
       <c r="F125" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126">
+    <row r="126" spans="1:6">
+      <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="B126">
+      <c r="B126" t="n">
         <v>6.7</v>
       </c>
-      <c r="C126">
+      <c r="C126" t="n">
         <v>3.3</v>
       </c>
-      <c r="D126">
+      <c r="D126" t="n">
         <v>5.7</v>
       </c>
-      <c r="E126">
+      <c r="E126" t="n">
         <v>2.1</v>
       </c>
       <c r="F126" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127">
+    <row r="127" spans="1:6">
+      <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="B127">
+      <c r="B127" t="n">
         <v>7.2</v>
       </c>
-      <c r="C127">
+      <c r="C127" t="n">
         <v>3.2</v>
       </c>
-      <c r="D127">
-        <v>6</v>
-      </c>
-      <c r="E127">
+      <c r="D127" t="n">
+        <v>6</v>
+      </c>
+      <c r="E127" t="n">
         <v>1.8</v>
       </c>
       <c r="F127" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128">
+    <row r="128" spans="1:6">
+      <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="B128">
+      <c r="B128" t="n">
         <v>6.2</v>
       </c>
-      <c r="C128">
+      <c r="C128" t="n">
         <v>2.8</v>
       </c>
-      <c r="D128">
+      <c r="D128" t="n">
         <v>4.8</v>
       </c>
-      <c r="E128">
+      <c r="E128" t="n">
         <v>1.8</v>
       </c>
       <c r="F128" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129">
+    <row r="129" spans="1:6">
+      <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="B129">
+      <c r="B129" t="n">
         <v>6.1</v>
       </c>
-      <c r="C129">
+      <c r="C129" t="n">
         <v>3</v>
       </c>
-      <c r="D129">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E129">
+      <c r="D129" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E129" t="n">
         <v>1.8</v>
       </c>
       <c r="F129" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130">
+    <row r="130" spans="1:6">
+      <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="B130">
+      <c r="B130" t="n">
         <v>6.4</v>
       </c>
-      <c r="C130">
+      <c r="C130" t="n">
         <v>2.8</v>
       </c>
-      <c r="D130">
+      <c r="D130" t="n">
         <v>5.6</v>
       </c>
-      <c r="E130">
+      <c r="E130" t="n">
         <v>2.1</v>
       </c>
       <c r="F130" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131">
+    <row r="131" spans="1:6">
+      <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="B131">
+      <c r="B131" t="n">
         <v>7.2</v>
       </c>
-      <c r="C131">
+      <c r="C131" t="n">
         <v>3</v>
       </c>
-      <c r="D131">
+      <c r="D131" t="n">
         <v>5.8</v>
       </c>
-      <c r="E131">
+      <c r="E131" t="n">
         <v>1.6</v>
       </c>
       <c r="F131" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132">
+    <row r="132" spans="1:6">
+      <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="B132">
+      <c r="B132" t="n">
         <v>7.4</v>
       </c>
-      <c r="C132">
+      <c r="C132" t="n">
         <v>2.8</v>
       </c>
-      <c r="D132">
+      <c r="D132" t="n">
         <v>6.1</v>
       </c>
-      <c r="E132">
+      <c r="E132" t="n">
         <v>1.9</v>
       </c>
       <c r="F132" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133">
+    <row r="133" spans="1:6">
+      <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="B133">
+      <c r="B133" t="n">
         <v>7.9</v>
       </c>
-      <c r="C133">
+      <c r="C133" t="n">
         <v>3.8</v>
       </c>
-      <c r="D133">
+      <c r="D133" t="n">
         <v>6.4</v>
       </c>
-      <c r="E133">
+      <c r="E133" t="n">
         <v>2</v>
       </c>
       <c r="F133" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A134">
+    <row r="134" spans="1:6">
+      <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="B134">
+      <c r="B134" t="n">
         <v>6.4</v>
       </c>
-      <c r="C134">
+      <c r="C134" t="n">
         <v>2.8</v>
       </c>
-      <c r="D134">
+      <c r="D134" t="n">
         <v>5.6</v>
       </c>
-      <c r="E134">
-        <v>2.2000000000000002</v>
+      <c r="E134" t="n">
+        <v>2.2</v>
       </c>
       <c r="F134" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135">
+    <row r="135" spans="1:6">
+      <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="B135">
+      <c r="B135" t="n">
         <v>6.3</v>
       </c>
-      <c r="C135">
+      <c r="C135" t="n">
         <v>2.8</v>
       </c>
-      <c r="D135">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E135">
+      <c r="D135" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E135" t="n">
         <v>1.5</v>
       </c>
       <c r="F135" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136">
+    <row r="136" spans="1:6">
+      <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="B136">
+      <c r="B136" t="n">
         <v>6.1</v>
       </c>
-      <c r="C136">
+      <c r="C136" t="n">
         <v>2.6</v>
       </c>
-      <c r="D136">
+      <c r="D136" t="n">
         <v>5.6</v>
       </c>
-      <c r="E136">
+      <c r="E136" t="n">
         <v>1.4</v>
       </c>
       <c r="F136" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137">
+    <row r="137" spans="1:6">
+      <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="B137">
+      <c r="B137" t="n">
         <v>7.7</v>
       </c>
-      <c r="C137">
+      <c r="C137" t="n">
         <v>3</v>
       </c>
-      <c r="D137">
+      <c r="D137" t="n">
         <v>6.1</v>
       </c>
-      <c r="E137">
-        <v>2.2999999999999998</v>
+      <c r="E137" t="n">
+        <v>2.3</v>
       </c>
       <c r="F137" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138">
+    <row r="138" spans="1:6">
+      <c r="A138" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="B138">
+      <c r="B138" t="n">
         <v>6.3</v>
       </c>
-      <c r="C138">
+      <c r="C138" t="n">
         <v>3.4</v>
       </c>
-      <c r="D138">
+      <c r="D138" t="n">
         <v>5.6</v>
       </c>
-      <c r="E138">
+      <c r="E138" t="n">
         <v>2.4</v>
       </c>
       <c r="F138" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139">
+    <row r="139" spans="1:6">
+      <c r="A139" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="B139">
+      <c r="B139" t="n">
         <v>6.4</v>
       </c>
-      <c r="C139">
+      <c r="C139" t="n">
         <v>3.1</v>
       </c>
-      <c r="D139">
+      <c r="D139" t="n">
         <v>5.5</v>
       </c>
-      <c r="E139">
+      <c r="E139" t="n">
         <v>1.8</v>
       </c>
       <c r="F139" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140">
+    <row r="140" spans="1:6">
+      <c r="A140" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="B140">
-        <v>6</v>
-      </c>
-      <c r="C140">
+      <c r="B140" t="n">
+        <v>6</v>
+      </c>
+      <c r="C140" t="n">
         <v>3</v>
       </c>
-      <c r="D140">
+      <c r="D140" t="n">
         <v>4.8</v>
       </c>
-      <c r="E140">
+      <c r="E140" t="n">
         <v>1.8</v>
       </c>
       <c r="F140" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A141">
+    <row r="141" spans="1:6">
+      <c r="A141" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="B141">
+      <c r="B141" t="n">
         <v>6.9</v>
       </c>
-      <c r="C141">
+      <c r="C141" t="n">
         <v>3.1</v>
       </c>
-      <c r="D141">
+      <c r="D141" t="n">
         <v>5.4</v>
       </c>
-      <c r="E141">
+      <c r="E141" t="n">
         <v>2.1</v>
       </c>
       <c r="F141" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142">
+    <row r="142" spans="1:6">
+      <c r="A142" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="B142">
+      <c r="B142" t="n">
         <v>6.7</v>
       </c>
-      <c r="C142">
+      <c r="C142" t="n">
         <v>3.1</v>
       </c>
-      <c r="D142">
+      <c r="D142" t="n">
         <v>5.6</v>
       </c>
-      <c r="E142">
+      <c r="E142" t="n">
         <v>2.4</v>
       </c>
       <c r="F142" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143">
+    <row r="143" spans="1:6">
+      <c r="A143" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="B143">
+      <c r="B143" t="n">
         <v>6.9</v>
       </c>
-      <c r="C143">
+      <c r="C143" t="n">
         <v>3.1</v>
       </c>
-      <c r="D143">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E143">
-        <v>2.2999999999999998</v>
+      <c r="D143" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E143" t="n">
+        <v>2.3</v>
       </c>
       <c r="F143" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144">
+    <row r="144" spans="1:6">
+      <c r="A144" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="B144">
+      <c r="B144" t="n">
         <v>5.8</v>
       </c>
-      <c r="C144">
+      <c r="C144" t="n">
         <v>2.7</v>
       </c>
-      <c r="D144">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E144">
+      <c r="D144" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E144" t="n">
         <v>1.9</v>
       </c>
       <c r="F144" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145">
+    <row r="145" spans="1:6">
+      <c r="A145" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="B145">
+      <c r="B145" t="n">
         <v>6.8</v>
       </c>
-      <c r="C145">
+      <c r="C145" t="n">
         <v>3.2</v>
       </c>
-      <c r="D145">
+      <c r="D145" t="n">
         <v>5.9</v>
       </c>
-      <c r="E145">
-        <v>2.2999999999999998</v>
+      <c r="E145" t="n">
+        <v>2.3</v>
       </c>
       <c r="F145" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146">
+    <row r="146" spans="1:6">
+      <c r="A146" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="B146">
+      <c r="B146" t="n">
         <v>6.7</v>
       </c>
-      <c r="C146">
+      <c r="C146" t="n">
         <v>3.3</v>
       </c>
-      <c r="D146">
+      <c r="D146" t="n">
         <v>5.7</v>
       </c>
-      <c r="E146">
+      <c r="E146" t="n">
         <v>2.5</v>
       </c>
       <c r="F146" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147">
+    <row r="147" spans="1:6">
+      <c r="A147" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="B147">
+      <c r="B147" t="n">
         <v>6.7</v>
       </c>
-      <c r="C147">
+      <c r="C147" t="n">
         <v>3</v>
       </c>
-      <c r="D147">
+      <c r="D147" t="n">
         <v>5.2</v>
       </c>
-      <c r="E147">
-        <v>2.2999999999999998</v>
+      <c r="E147" t="n">
+        <v>2.3</v>
       </c>
       <c r="F147" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A148">
+    <row r="148" spans="1:6">
+      <c r="A148" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="B148">
+      <c r="B148" t="n">
         <v>6.3</v>
       </c>
-      <c r="C148">
+      <c r="C148" t="n">
         <v>2.5</v>
       </c>
-      <c r="D148">
-        <v>5</v>
-      </c>
-      <c r="E148">
+      <c r="D148" t="n">
+        <v>5</v>
+      </c>
+      <c r="E148" t="n">
         <v>1.9</v>
       </c>
       <c r="F148" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149">
+    <row r="149" spans="1:6">
+      <c r="A149" s="1" t="n">
         <v>147</v>
       </c>
-      <c r="B149">
+      <c r="B149" t="n">
         <v>6.5</v>
       </c>
-      <c r="C149">
+      <c r="C149" t="n">
         <v>3</v>
       </c>
-      <c r="D149">
+      <c r="D149" t="n">
         <v>5.2</v>
       </c>
-      <c r="E149">
+      <c r="E149" t="n">
         <v>2</v>
       </c>
       <c r="F149" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150">
+    <row r="150" spans="1:6">
+      <c r="A150" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="B150">
+      <c r="B150" t="n">
         <v>6.2</v>
       </c>
-      <c r="C150">
+      <c r="C150" t="n">
         <v>3.4</v>
       </c>
-      <c r="D150">
+      <c r="D150" t="n">
         <v>5.4</v>
       </c>
-      <c r="E150">
-        <v>2.2999999999999998</v>
+      <c r="E150" t="n">
+        <v>2.3</v>
       </c>
       <c r="F150" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151">
+    <row r="151" spans="1:6">
+      <c r="A151" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="B151">
+      <c r="B151" t="n">
         <v>5.9</v>
       </c>
-      <c r="C151">
+      <c r="C151" t="n">
         <v>3</v>
       </c>
-      <c r="D151">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E151">
+      <c r="D151" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E151" t="n">
         <v>1.8</v>
       </c>
       <c r="F151" t="s">
@@ -3389,6 +3413,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>